<commit_message>
General diss work and making test plot files
</commit_message>
<xml_diff>
--- a/Analysis/High level/comparisons.xlsx
+++ b/Analysis/High level/comparisons.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="52">
   <si>
     <t>0-&gt;1</t>
   </si>
@@ -170,6 +170,9 @@
   <si>
     <t>not put in graph because results are weird</t>
   </si>
+  <si>
+    <t>median</t>
+  </si>
 </sst>
 </file>
 
@@ -5554,11 +5557,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="83548032"/>
-        <c:axId val="84928000"/>
+        <c:axId val="46167168"/>
+        <c:axId val="46168704"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="83548032"/>
+        <c:axId val="46167168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5568,7 +5571,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84928000"/>
+        <c:crossAx val="46168704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5576,7 +5579,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="84928000"/>
+        <c:axId val="46168704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -5588,7 +5591,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83548032"/>
+        <c:crossAx val="46167168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7827,11 +7830,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="84971904"/>
-        <c:axId val="84973824"/>
+        <c:axId val="46077056"/>
+        <c:axId val="46078592"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="84971904"/>
+        <c:axId val="46077056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7841,7 +7844,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84973824"/>
+        <c:crossAx val="46078592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7849,7 +7852,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="84973824"/>
+        <c:axId val="46078592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7860,13 +7863,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84971904"/>
+        <c:crossAx val="46077056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -15713,11 +15717,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="83819136"/>
-        <c:axId val="85062016"/>
+        <c:axId val="46128512"/>
+        <c:axId val="46134400"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="83819136"/>
+        <c:axId val="46128512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15727,7 +15731,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85062016"/>
+        <c:crossAx val="46134400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15735,7 +15739,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="85062016"/>
+        <c:axId val="46134400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15746,7 +15750,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83819136"/>
+        <c:crossAx val="46128512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -16150,16 +16154,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:SZ245"/>
+  <dimension ref="A1:SZ247"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A230" workbookViewId="0">
-      <selection activeCell="A248" sqref="A248"/>
+    <sheetView tabSelected="1" topLeftCell="A226" workbookViewId="0">
+      <selection activeCell="D248" sqref="D248"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42" customWidth="1"/>
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:188" x14ac:dyDescent="0.25">
@@ -86364,6 +86369,2089 @@
       <c r="SZ245">
         <f t="shared" si="550"/>
         <v>1</v>
+      </c>
+    </row>
+    <row r="246" spans="2:520" x14ac:dyDescent="0.25">
+      <c r="B246" t="s">
+        <v>51</v>
+      </c>
+      <c r="C246">
+        <f>MEDIAN(C238:C243)</f>
+        <v>236</v>
+      </c>
+      <c r="D246">
+        <f t="shared" ref="D246:BO246" si="551">MEDIAN(D238:D243)</f>
+        <v>301</v>
+      </c>
+      <c r="E246">
+        <f t="shared" si="551"/>
+        <v>305</v>
+      </c>
+      <c r="F246">
+        <f t="shared" si="551"/>
+        <v>305</v>
+      </c>
+      <c r="G246">
+        <f t="shared" si="551"/>
+        <v>305</v>
+      </c>
+      <c r="H246">
+        <f t="shared" si="551"/>
+        <v>305.5</v>
+      </c>
+      <c r="I246">
+        <f t="shared" si="551"/>
+        <v>306</v>
+      </c>
+      <c r="J246">
+        <f t="shared" si="551"/>
+        <v>306.5</v>
+      </c>
+      <c r="K246">
+        <f t="shared" si="551"/>
+        <v>306.5</v>
+      </c>
+      <c r="L246">
+        <f t="shared" si="551"/>
+        <v>307</v>
+      </c>
+      <c r="M246">
+        <f t="shared" si="551"/>
+        <v>307.5</v>
+      </c>
+      <c r="N246">
+        <f t="shared" si="551"/>
+        <v>308</v>
+      </c>
+      <c r="O246">
+        <f t="shared" si="551"/>
+        <v>309</v>
+      </c>
+      <c r="P246">
+        <f t="shared" si="551"/>
+        <v>309.5</v>
+      </c>
+      <c r="Q246">
+        <f t="shared" si="551"/>
+        <v>309.5</v>
+      </c>
+      <c r="R246">
+        <f t="shared" si="551"/>
+        <v>310</v>
+      </c>
+      <c r="S246">
+        <f t="shared" si="551"/>
+        <v>310</v>
+      </c>
+      <c r="T246">
+        <f t="shared" si="551"/>
+        <v>310.5</v>
+      </c>
+      <c r="U246">
+        <f t="shared" si="551"/>
+        <v>311</v>
+      </c>
+      <c r="V246">
+        <f t="shared" si="551"/>
+        <v>312</v>
+      </c>
+      <c r="W246">
+        <f t="shared" si="551"/>
+        <v>312.5</v>
+      </c>
+      <c r="X246">
+        <f t="shared" si="551"/>
+        <v>313</v>
+      </c>
+      <c r="Y246">
+        <f t="shared" si="551"/>
+        <v>314.5</v>
+      </c>
+      <c r="Z246">
+        <f t="shared" si="551"/>
+        <v>315.5</v>
+      </c>
+      <c r="AA246">
+        <f t="shared" si="551"/>
+        <v>316</v>
+      </c>
+      <c r="AB246">
+        <f t="shared" si="551"/>
+        <v>316.5</v>
+      </c>
+      <c r="AC246">
+        <f t="shared" si="551"/>
+        <v>317</v>
+      </c>
+      <c r="AD246">
+        <f t="shared" si="551"/>
+        <v>317.5</v>
+      </c>
+      <c r="AE246">
+        <f t="shared" si="551"/>
+        <v>318</v>
+      </c>
+      <c r="AF246">
+        <f t="shared" si="551"/>
+        <v>318.5</v>
+      </c>
+      <c r="AG246">
+        <f t="shared" si="551"/>
+        <v>319</v>
+      </c>
+      <c r="AH246">
+        <f t="shared" si="551"/>
+        <v>319.5</v>
+      </c>
+      <c r="AI246">
+        <f t="shared" si="551"/>
+        <v>319.5</v>
+      </c>
+      <c r="AJ246">
+        <f t="shared" si="551"/>
+        <v>320</v>
+      </c>
+      <c r="AK246">
+        <f t="shared" si="551"/>
+        <v>320.5</v>
+      </c>
+      <c r="AL246">
+        <f t="shared" si="551"/>
+        <v>320.5</v>
+      </c>
+      <c r="AM246">
+        <f t="shared" si="551"/>
+        <v>321</v>
+      </c>
+      <c r="AN246">
+        <f t="shared" si="551"/>
+        <v>321.5</v>
+      </c>
+      <c r="AO246">
+        <f t="shared" si="551"/>
+        <v>322</v>
+      </c>
+      <c r="AP246">
+        <f t="shared" si="551"/>
+        <v>322.5</v>
+      </c>
+      <c r="AQ246">
+        <f t="shared" si="551"/>
+        <v>323</v>
+      </c>
+      <c r="AR246">
+        <f t="shared" si="551"/>
+        <v>323.5</v>
+      </c>
+      <c r="AS246">
+        <f t="shared" si="551"/>
+        <v>324</v>
+      </c>
+      <c r="AT246">
+        <f t="shared" si="551"/>
+        <v>324.5</v>
+      </c>
+      <c r="AU246">
+        <f t="shared" si="551"/>
+        <v>324.5</v>
+      </c>
+      <c r="AV246">
+        <f t="shared" si="551"/>
+        <v>325</v>
+      </c>
+      <c r="AW246">
+        <f t="shared" si="551"/>
+        <v>326</v>
+      </c>
+      <c r="AX246">
+        <f t="shared" si="551"/>
+        <v>326.5</v>
+      </c>
+      <c r="AY246">
+        <f t="shared" si="551"/>
+        <v>327</v>
+      </c>
+      <c r="AZ246">
+        <f t="shared" si="551"/>
+        <v>327.5</v>
+      </c>
+      <c r="BA246">
+        <f t="shared" si="551"/>
+        <v>328</v>
+      </c>
+      <c r="BB246">
+        <f t="shared" si="551"/>
+        <v>329</v>
+      </c>
+      <c r="BC246">
+        <f t="shared" si="551"/>
+        <v>329.5</v>
+      </c>
+      <c r="BD246">
+        <f t="shared" si="551"/>
+        <v>330</v>
+      </c>
+      <c r="BE246">
+        <f t="shared" si="551"/>
+        <v>330.5</v>
+      </c>
+      <c r="BF246">
+        <f t="shared" si="551"/>
+        <v>331</v>
+      </c>
+      <c r="BG246">
+        <f t="shared" si="551"/>
+        <v>331</v>
+      </c>
+      <c r="BH246">
+        <f t="shared" si="551"/>
+        <v>331.5</v>
+      </c>
+      <c r="BI246">
+        <f t="shared" si="551"/>
+        <v>332</v>
+      </c>
+      <c r="BJ246">
+        <f t="shared" si="551"/>
+        <v>332</v>
+      </c>
+      <c r="BK246">
+        <f t="shared" si="551"/>
+        <v>332</v>
+      </c>
+      <c r="BL246">
+        <f t="shared" si="551"/>
+        <v>332</v>
+      </c>
+      <c r="BM246">
+        <f t="shared" si="551"/>
+        <v>332</v>
+      </c>
+      <c r="BN246">
+        <f t="shared" si="551"/>
+        <v>332</v>
+      </c>
+      <c r="BO246">
+        <f t="shared" si="551"/>
+        <v>332</v>
+      </c>
+      <c r="BP246">
+        <f t="shared" ref="BP246:EA246" si="552">MEDIAN(BP238:BP243)</f>
+        <v>332</v>
+      </c>
+      <c r="BQ246">
+        <f t="shared" si="552"/>
+        <v>332</v>
+      </c>
+      <c r="BR246">
+        <f t="shared" si="552"/>
+        <v>332</v>
+      </c>
+      <c r="BS246">
+        <f t="shared" si="552"/>
+        <v>332</v>
+      </c>
+      <c r="BT246">
+        <f t="shared" si="552"/>
+        <v>332</v>
+      </c>
+      <c r="BU246">
+        <f t="shared" si="552"/>
+        <v>332</v>
+      </c>
+      <c r="BV246">
+        <f t="shared" si="552"/>
+        <v>332</v>
+      </c>
+      <c r="BW246">
+        <f t="shared" si="552"/>
+        <v>332</v>
+      </c>
+      <c r="BX246">
+        <f t="shared" si="552"/>
+        <v>332</v>
+      </c>
+      <c r="BY246">
+        <f t="shared" si="552"/>
+        <v>332</v>
+      </c>
+      <c r="BZ246">
+        <f t="shared" si="552"/>
+        <v>332</v>
+      </c>
+      <c r="CA246">
+        <f t="shared" si="552"/>
+        <v>332</v>
+      </c>
+      <c r="CB246">
+        <f t="shared" si="552"/>
+        <v>332</v>
+      </c>
+      <c r="CC246">
+        <f t="shared" si="552"/>
+        <v>332</v>
+      </c>
+      <c r="CD246">
+        <f t="shared" si="552"/>
+        <v>332</v>
+      </c>
+      <c r="CE246">
+        <f t="shared" si="552"/>
+        <v>332</v>
+      </c>
+      <c r="CF246">
+        <f t="shared" si="552"/>
+        <v>332</v>
+      </c>
+      <c r="CG246">
+        <f t="shared" si="552"/>
+        <v>332</v>
+      </c>
+      <c r="CH246">
+        <f t="shared" si="552"/>
+        <v>332</v>
+      </c>
+      <c r="CI246">
+        <f t="shared" si="552"/>
+        <v>332</v>
+      </c>
+      <c r="CJ246">
+        <f t="shared" si="552"/>
+        <v>332</v>
+      </c>
+      <c r="CK246">
+        <f t="shared" si="552"/>
+        <v>332</v>
+      </c>
+      <c r="CL246">
+        <f t="shared" si="552"/>
+        <v>332</v>
+      </c>
+      <c r="CM246">
+        <f t="shared" si="552"/>
+        <v>332</v>
+      </c>
+      <c r="CN246">
+        <f t="shared" si="552"/>
+        <v>332</v>
+      </c>
+      <c r="CO246">
+        <f t="shared" si="552"/>
+        <v>332</v>
+      </c>
+      <c r="CP246">
+        <f t="shared" si="552"/>
+        <v>332</v>
+      </c>
+      <c r="CQ246">
+        <f t="shared" si="552"/>
+        <v>332</v>
+      </c>
+      <c r="CR246">
+        <f t="shared" si="552"/>
+        <v>332</v>
+      </c>
+      <c r="CS246">
+        <f t="shared" si="552"/>
+        <v>332</v>
+      </c>
+      <c r="CT246">
+        <f t="shared" si="552"/>
+        <v>332</v>
+      </c>
+      <c r="CU246">
+        <f t="shared" si="552"/>
+        <v>332</v>
+      </c>
+      <c r="CV246">
+        <f t="shared" si="552"/>
+        <v>332</v>
+      </c>
+      <c r="CW246">
+        <f t="shared" si="552"/>
+        <v>332</v>
+      </c>
+      <c r="CX246">
+        <f t="shared" si="552"/>
+        <v>332</v>
+      </c>
+      <c r="CY246">
+        <f t="shared" si="552"/>
+        <v>332</v>
+      </c>
+      <c r="CZ246">
+        <f t="shared" si="552"/>
+        <v>332</v>
+      </c>
+      <c r="DA246">
+        <f t="shared" si="552"/>
+        <v>332</v>
+      </c>
+      <c r="DB246">
+        <f t="shared" si="552"/>
+        <v>332</v>
+      </c>
+      <c r="DC246">
+        <f t="shared" si="552"/>
+        <v>332</v>
+      </c>
+      <c r="DD246">
+        <f t="shared" si="552"/>
+        <v>332</v>
+      </c>
+      <c r="DE246">
+        <f t="shared" si="552"/>
+        <v>332</v>
+      </c>
+      <c r="DF246">
+        <f t="shared" si="552"/>
+        <v>332</v>
+      </c>
+      <c r="DG246">
+        <f t="shared" si="552"/>
+        <v>332</v>
+      </c>
+      <c r="DH246">
+        <f t="shared" si="552"/>
+        <v>332</v>
+      </c>
+      <c r="DI246">
+        <f t="shared" si="552"/>
+        <v>332</v>
+      </c>
+      <c r="DJ246">
+        <f t="shared" si="552"/>
+        <v>332</v>
+      </c>
+      <c r="DK246">
+        <f t="shared" si="552"/>
+        <v>332</v>
+      </c>
+      <c r="DL246">
+        <f t="shared" si="552"/>
+        <v>332</v>
+      </c>
+      <c r="DM246">
+        <f t="shared" si="552"/>
+        <v>332</v>
+      </c>
+      <c r="DN246">
+        <f t="shared" si="552"/>
+        <v>332</v>
+      </c>
+      <c r="DO246">
+        <f t="shared" si="552"/>
+        <v>332</v>
+      </c>
+      <c r="DP246">
+        <f t="shared" si="552"/>
+        <v>332</v>
+      </c>
+      <c r="DQ246">
+        <f t="shared" si="552"/>
+        <v>332</v>
+      </c>
+      <c r="DR246">
+        <f t="shared" si="552"/>
+        <v>332</v>
+      </c>
+      <c r="DS246">
+        <f t="shared" si="552"/>
+        <v>332</v>
+      </c>
+      <c r="DT246">
+        <f t="shared" si="552"/>
+        <v>332</v>
+      </c>
+      <c r="DU246">
+        <f t="shared" si="552"/>
+        <v>332</v>
+      </c>
+      <c r="DV246">
+        <f t="shared" si="552"/>
+        <v>332</v>
+      </c>
+      <c r="DW246">
+        <f t="shared" si="552"/>
+        <v>332</v>
+      </c>
+      <c r="DX246">
+        <f t="shared" si="552"/>
+        <v>332</v>
+      </c>
+      <c r="DY246">
+        <f t="shared" si="552"/>
+        <v>332</v>
+      </c>
+      <c r="DZ246">
+        <f t="shared" si="552"/>
+        <v>332</v>
+      </c>
+      <c r="EA246">
+        <f t="shared" si="552"/>
+        <v>332</v>
+      </c>
+      <c r="EB246">
+        <f t="shared" ref="EB246:GM246" si="553">MEDIAN(EB238:EB243)</f>
+        <v>332</v>
+      </c>
+      <c r="EC246">
+        <f t="shared" si="553"/>
+        <v>332</v>
+      </c>
+      <c r="ED246">
+        <f t="shared" si="553"/>
+        <v>332</v>
+      </c>
+      <c r="EE246">
+        <f t="shared" si="553"/>
+        <v>332</v>
+      </c>
+      <c r="EF246">
+        <f t="shared" si="553"/>
+        <v>332</v>
+      </c>
+      <c r="EG246">
+        <f t="shared" si="553"/>
+        <v>332</v>
+      </c>
+      <c r="EH246">
+        <f t="shared" si="553"/>
+        <v>332</v>
+      </c>
+      <c r="EI246">
+        <f t="shared" si="553"/>
+        <v>332</v>
+      </c>
+      <c r="EJ246">
+        <f t="shared" si="553"/>
+        <v>332</v>
+      </c>
+      <c r="EK246">
+        <f t="shared" si="553"/>
+        <v>332</v>
+      </c>
+      <c r="EL246">
+        <f t="shared" si="553"/>
+        <v>332</v>
+      </c>
+      <c r="EM246">
+        <f t="shared" si="553"/>
+        <v>332</v>
+      </c>
+      <c r="EN246">
+        <f t="shared" si="553"/>
+        <v>332</v>
+      </c>
+      <c r="EO246">
+        <f t="shared" si="553"/>
+        <v>332</v>
+      </c>
+      <c r="EP246">
+        <f t="shared" si="553"/>
+        <v>332</v>
+      </c>
+      <c r="EQ246">
+        <f t="shared" si="553"/>
+        <v>332</v>
+      </c>
+      <c r="ER246">
+        <f t="shared" si="553"/>
+        <v>332</v>
+      </c>
+      <c r="ES246">
+        <f t="shared" si="553"/>
+        <v>332</v>
+      </c>
+      <c r="ET246">
+        <f t="shared" si="553"/>
+        <v>332</v>
+      </c>
+      <c r="EU246">
+        <f t="shared" si="553"/>
+        <v>332</v>
+      </c>
+      <c r="EV246">
+        <f t="shared" si="553"/>
+        <v>332</v>
+      </c>
+      <c r="EW246">
+        <f t="shared" si="553"/>
+        <v>332</v>
+      </c>
+      <c r="EX246">
+        <f t="shared" si="553"/>
+        <v>332</v>
+      </c>
+      <c r="EY246">
+        <f t="shared" si="553"/>
+        <v>332</v>
+      </c>
+      <c r="EZ246">
+        <f t="shared" si="553"/>
+        <v>332</v>
+      </c>
+      <c r="FA246">
+        <f t="shared" si="553"/>
+        <v>332</v>
+      </c>
+      <c r="FB246">
+        <f t="shared" si="553"/>
+        <v>332</v>
+      </c>
+      <c r="FC246">
+        <f t="shared" si="553"/>
+        <v>332</v>
+      </c>
+      <c r="FD246">
+        <f t="shared" si="553"/>
+        <v>332</v>
+      </c>
+      <c r="FE246">
+        <f t="shared" si="553"/>
+        <v>332</v>
+      </c>
+      <c r="FF246">
+        <f t="shared" si="553"/>
+        <v>332</v>
+      </c>
+      <c r="FG246">
+        <f t="shared" si="553"/>
+        <v>332</v>
+      </c>
+      <c r="FH246">
+        <f t="shared" si="553"/>
+        <v>332</v>
+      </c>
+      <c r="FI246">
+        <f t="shared" si="553"/>
+        <v>332</v>
+      </c>
+      <c r="FJ246">
+        <f t="shared" si="553"/>
+        <v>332</v>
+      </c>
+      <c r="FK246">
+        <f t="shared" si="553"/>
+        <v>332</v>
+      </c>
+      <c r="FL246">
+        <f t="shared" si="553"/>
+        <v>332</v>
+      </c>
+      <c r="FM246">
+        <f t="shared" si="553"/>
+        <v>332</v>
+      </c>
+      <c r="FN246">
+        <f t="shared" si="553"/>
+        <v>332</v>
+      </c>
+      <c r="FO246">
+        <f t="shared" si="553"/>
+        <v>332</v>
+      </c>
+      <c r="FP246">
+        <f t="shared" si="553"/>
+        <v>332</v>
+      </c>
+      <c r="FQ246">
+        <f t="shared" si="553"/>
+        <v>332</v>
+      </c>
+      <c r="FR246">
+        <f t="shared" si="553"/>
+        <v>332</v>
+      </c>
+      <c r="FS246">
+        <f t="shared" si="553"/>
+        <v>332</v>
+      </c>
+      <c r="FT246">
+        <f t="shared" si="553"/>
+        <v>332</v>
+      </c>
+      <c r="FU246">
+        <f t="shared" si="553"/>
+        <v>332</v>
+      </c>
+      <c r="FV246">
+        <f t="shared" si="553"/>
+        <v>332</v>
+      </c>
+      <c r="FW246">
+        <f t="shared" si="553"/>
+        <v>332</v>
+      </c>
+      <c r="FX246">
+        <f t="shared" si="553"/>
+        <v>332</v>
+      </c>
+      <c r="FY246">
+        <f t="shared" si="553"/>
+        <v>332</v>
+      </c>
+      <c r="FZ246">
+        <f t="shared" si="553"/>
+        <v>332</v>
+      </c>
+      <c r="GA246">
+        <f t="shared" si="553"/>
+        <v>332</v>
+      </c>
+      <c r="GB246">
+        <f t="shared" si="553"/>
+        <v>332</v>
+      </c>
+      <c r="GC246">
+        <f t="shared" si="553"/>
+        <v>332</v>
+      </c>
+      <c r="GD246">
+        <f t="shared" si="553"/>
+        <v>332</v>
+      </c>
+      <c r="GE246">
+        <f t="shared" si="553"/>
+        <v>332</v>
+      </c>
+      <c r="GF246">
+        <f t="shared" si="553"/>
+        <v>332</v>
+      </c>
+      <c r="GG246">
+        <f t="shared" si="553"/>
+        <v>332</v>
+      </c>
+      <c r="GH246">
+        <f t="shared" si="553"/>
+        <v>332</v>
+      </c>
+      <c r="GI246">
+        <f t="shared" si="553"/>
+        <v>332</v>
+      </c>
+      <c r="GJ246">
+        <f t="shared" si="553"/>
+        <v>332</v>
+      </c>
+      <c r="GK246">
+        <f t="shared" si="553"/>
+        <v>332</v>
+      </c>
+      <c r="GL246">
+        <f t="shared" si="553"/>
+        <v>332</v>
+      </c>
+      <c r="GM246">
+        <f t="shared" si="553"/>
+        <v>332</v>
+      </c>
+      <c r="GN246">
+        <f t="shared" ref="GN246:IY246" si="554">MEDIAN(GN238:GN243)</f>
+        <v>332</v>
+      </c>
+      <c r="GO246">
+        <f t="shared" si="554"/>
+        <v>332</v>
+      </c>
+      <c r="GP246">
+        <f t="shared" si="554"/>
+        <v>332</v>
+      </c>
+      <c r="GQ246">
+        <f t="shared" si="554"/>
+        <v>332</v>
+      </c>
+      <c r="GR246">
+        <f t="shared" si="554"/>
+        <v>332</v>
+      </c>
+      <c r="GS246">
+        <f t="shared" si="554"/>
+        <v>332</v>
+      </c>
+      <c r="GT246">
+        <f t="shared" si="554"/>
+        <v>332</v>
+      </c>
+      <c r="GU246">
+        <f t="shared" si="554"/>
+        <v>332</v>
+      </c>
+      <c r="GV246">
+        <f t="shared" si="554"/>
+        <v>332</v>
+      </c>
+      <c r="GW246">
+        <f t="shared" si="554"/>
+        <v>332</v>
+      </c>
+      <c r="GX246">
+        <f t="shared" si="554"/>
+        <v>332</v>
+      </c>
+      <c r="GY246">
+        <f t="shared" si="554"/>
+        <v>332</v>
+      </c>
+      <c r="GZ246">
+        <f t="shared" si="554"/>
+        <v>332</v>
+      </c>
+      <c r="HA246">
+        <f t="shared" si="554"/>
+        <v>332</v>
+      </c>
+      <c r="HB246">
+        <f t="shared" si="554"/>
+        <v>332</v>
+      </c>
+      <c r="HC246">
+        <f t="shared" si="554"/>
+        <v>332</v>
+      </c>
+      <c r="HD246">
+        <f t="shared" si="554"/>
+        <v>332</v>
+      </c>
+      <c r="HE246">
+        <f t="shared" si="554"/>
+        <v>332</v>
+      </c>
+      <c r="HF246">
+        <f t="shared" si="554"/>
+        <v>332</v>
+      </c>
+      <c r="HG246">
+        <f t="shared" si="554"/>
+        <v>332</v>
+      </c>
+      <c r="HH246">
+        <f t="shared" si="554"/>
+        <v>332</v>
+      </c>
+      <c r="HI246">
+        <f t="shared" si="554"/>
+        <v>332</v>
+      </c>
+      <c r="HJ246">
+        <f t="shared" si="554"/>
+        <v>332</v>
+      </c>
+      <c r="HK246">
+        <f t="shared" si="554"/>
+        <v>332</v>
+      </c>
+      <c r="HL246">
+        <f t="shared" si="554"/>
+        <v>332</v>
+      </c>
+      <c r="HM246">
+        <f t="shared" si="554"/>
+        <v>332</v>
+      </c>
+      <c r="HN246">
+        <f t="shared" si="554"/>
+        <v>332</v>
+      </c>
+      <c r="HO246">
+        <f t="shared" si="554"/>
+        <v>332</v>
+      </c>
+      <c r="HP246">
+        <f t="shared" si="554"/>
+        <v>332</v>
+      </c>
+      <c r="HQ246">
+        <f t="shared" si="554"/>
+        <v>332</v>
+      </c>
+      <c r="HR246">
+        <f t="shared" si="554"/>
+        <v>332</v>
+      </c>
+      <c r="HS246">
+        <f t="shared" si="554"/>
+        <v>332</v>
+      </c>
+      <c r="HT246">
+        <f t="shared" si="554"/>
+        <v>332</v>
+      </c>
+      <c r="HU246">
+        <f t="shared" si="554"/>
+        <v>332</v>
+      </c>
+      <c r="HV246">
+        <f t="shared" si="554"/>
+        <v>332</v>
+      </c>
+      <c r="HW246">
+        <f t="shared" si="554"/>
+        <v>332</v>
+      </c>
+      <c r="HX246">
+        <f t="shared" si="554"/>
+        <v>332</v>
+      </c>
+      <c r="HY246">
+        <f t="shared" si="554"/>
+        <v>332</v>
+      </c>
+      <c r="HZ246">
+        <f t="shared" si="554"/>
+        <v>332</v>
+      </c>
+      <c r="IA246">
+        <f t="shared" si="554"/>
+        <v>332</v>
+      </c>
+      <c r="IB246">
+        <f t="shared" si="554"/>
+        <v>332</v>
+      </c>
+      <c r="IC246">
+        <f t="shared" si="554"/>
+        <v>332</v>
+      </c>
+      <c r="ID246">
+        <f t="shared" si="554"/>
+        <v>332</v>
+      </c>
+      <c r="IE246">
+        <f t="shared" si="554"/>
+        <v>332</v>
+      </c>
+      <c r="IF246">
+        <f t="shared" si="554"/>
+        <v>332</v>
+      </c>
+      <c r="IG246">
+        <f t="shared" si="554"/>
+        <v>332</v>
+      </c>
+      <c r="IH246">
+        <f t="shared" si="554"/>
+        <v>332</v>
+      </c>
+      <c r="II246">
+        <f t="shared" si="554"/>
+        <v>332</v>
+      </c>
+      <c r="IJ246">
+        <f t="shared" si="554"/>
+        <v>332</v>
+      </c>
+      <c r="IK246">
+        <f t="shared" si="554"/>
+        <v>332</v>
+      </c>
+      <c r="IL246">
+        <f t="shared" si="554"/>
+        <v>332</v>
+      </c>
+      <c r="IM246">
+        <f t="shared" si="554"/>
+        <v>332</v>
+      </c>
+      <c r="IN246">
+        <f t="shared" si="554"/>
+        <v>332</v>
+      </c>
+      <c r="IO246">
+        <f t="shared" si="554"/>
+        <v>332</v>
+      </c>
+      <c r="IP246">
+        <f t="shared" si="554"/>
+        <v>332</v>
+      </c>
+      <c r="IQ246">
+        <f t="shared" si="554"/>
+        <v>332</v>
+      </c>
+      <c r="IR246">
+        <f t="shared" si="554"/>
+        <v>332</v>
+      </c>
+      <c r="IS246">
+        <f t="shared" si="554"/>
+        <v>332</v>
+      </c>
+      <c r="IT246">
+        <f t="shared" si="554"/>
+        <v>332</v>
+      </c>
+      <c r="IU246">
+        <f t="shared" si="554"/>
+        <v>332</v>
+      </c>
+      <c r="IV246">
+        <f t="shared" si="554"/>
+        <v>332</v>
+      </c>
+      <c r="IW246">
+        <f t="shared" si="554"/>
+        <v>332</v>
+      </c>
+      <c r="IX246">
+        <f t="shared" si="554"/>
+        <v>332</v>
+      </c>
+      <c r="IY246">
+        <f t="shared" si="554"/>
+        <v>332</v>
+      </c>
+      <c r="IZ246">
+        <f t="shared" ref="IZ246:LK246" si="555">MEDIAN(IZ238:IZ243)</f>
+        <v>332</v>
+      </c>
+      <c r="JA246">
+        <f t="shared" si="555"/>
+        <v>332</v>
+      </c>
+      <c r="JB246">
+        <f t="shared" si="555"/>
+        <v>332</v>
+      </c>
+      <c r="JC246">
+        <f t="shared" si="555"/>
+        <v>332</v>
+      </c>
+      <c r="JD246">
+        <f t="shared" si="555"/>
+        <v>332</v>
+      </c>
+      <c r="JE246">
+        <f t="shared" si="555"/>
+        <v>332</v>
+      </c>
+      <c r="JF246">
+        <f t="shared" si="555"/>
+        <v>332</v>
+      </c>
+      <c r="JG246">
+        <f t="shared" si="555"/>
+        <v>332</v>
+      </c>
+      <c r="JH246">
+        <f t="shared" si="555"/>
+        <v>332</v>
+      </c>
+      <c r="JI246">
+        <f t="shared" si="555"/>
+        <v>332</v>
+      </c>
+      <c r="JJ246">
+        <f t="shared" si="555"/>
+        <v>332</v>
+      </c>
+      <c r="JK246">
+        <f t="shared" si="555"/>
+        <v>332</v>
+      </c>
+      <c r="JL246">
+        <f t="shared" si="555"/>
+        <v>332</v>
+      </c>
+      <c r="JM246">
+        <f t="shared" si="555"/>
+        <v>332</v>
+      </c>
+      <c r="JN246">
+        <f t="shared" si="555"/>
+        <v>332</v>
+      </c>
+      <c r="JO246">
+        <f t="shared" si="555"/>
+        <v>332</v>
+      </c>
+      <c r="JP246">
+        <f t="shared" si="555"/>
+        <v>332</v>
+      </c>
+      <c r="JQ246">
+        <f t="shared" si="555"/>
+        <v>332</v>
+      </c>
+      <c r="JR246">
+        <f t="shared" si="555"/>
+        <v>332</v>
+      </c>
+      <c r="JS246">
+        <f t="shared" si="555"/>
+        <v>332</v>
+      </c>
+      <c r="JT246">
+        <f t="shared" si="555"/>
+        <v>332</v>
+      </c>
+      <c r="JU246">
+        <f t="shared" si="555"/>
+        <v>332</v>
+      </c>
+      <c r="JV246">
+        <f t="shared" si="555"/>
+        <v>332</v>
+      </c>
+      <c r="JW246">
+        <f t="shared" si="555"/>
+        <v>332</v>
+      </c>
+      <c r="JX246">
+        <f t="shared" si="555"/>
+        <v>332</v>
+      </c>
+      <c r="JY246">
+        <f t="shared" si="555"/>
+        <v>332</v>
+      </c>
+      <c r="JZ246">
+        <f t="shared" si="555"/>
+        <v>332</v>
+      </c>
+      <c r="KA246">
+        <f t="shared" si="555"/>
+        <v>332</v>
+      </c>
+      <c r="KB246">
+        <f t="shared" si="555"/>
+        <v>332</v>
+      </c>
+      <c r="KC246">
+        <f t="shared" si="555"/>
+        <v>332</v>
+      </c>
+      <c r="KD246">
+        <f t="shared" si="555"/>
+        <v>332</v>
+      </c>
+      <c r="KE246">
+        <f t="shared" si="555"/>
+        <v>332</v>
+      </c>
+      <c r="KF246">
+        <f t="shared" si="555"/>
+        <v>332</v>
+      </c>
+      <c r="KG246">
+        <f t="shared" si="555"/>
+        <v>332</v>
+      </c>
+      <c r="KH246">
+        <f t="shared" si="555"/>
+        <v>332</v>
+      </c>
+      <c r="KI246">
+        <f t="shared" si="555"/>
+        <v>332</v>
+      </c>
+      <c r="KJ246">
+        <f t="shared" si="555"/>
+        <v>332</v>
+      </c>
+      <c r="KK246">
+        <f t="shared" si="555"/>
+        <v>332</v>
+      </c>
+      <c r="KL246">
+        <f t="shared" si="555"/>
+        <v>332</v>
+      </c>
+      <c r="KM246">
+        <f t="shared" si="555"/>
+        <v>332</v>
+      </c>
+      <c r="KN246">
+        <f t="shared" si="555"/>
+        <v>332</v>
+      </c>
+      <c r="KO246">
+        <f t="shared" si="555"/>
+        <v>332</v>
+      </c>
+      <c r="KP246">
+        <f t="shared" si="555"/>
+        <v>332</v>
+      </c>
+      <c r="KQ246">
+        <f t="shared" si="555"/>
+        <v>332</v>
+      </c>
+      <c r="KR246">
+        <f t="shared" si="555"/>
+        <v>332</v>
+      </c>
+      <c r="KS246">
+        <f t="shared" si="555"/>
+        <v>332</v>
+      </c>
+      <c r="KT246">
+        <f t="shared" si="555"/>
+        <v>332</v>
+      </c>
+      <c r="KU246">
+        <f t="shared" si="555"/>
+        <v>332</v>
+      </c>
+      <c r="KV246">
+        <f t="shared" si="555"/>
+        <v>332</v>
+      </c>
+      <c r="KW246">
+        <f t="shared" si="555"/>
+        <v>332</v>
+      </c>
+      <c r="KX246">
+        <f t="shared" si="555"/>
+        <v>332</v>
+      </c>
+      <c r="KY246">
+        <f t="shared" si="555"/>
+        <v>332</v>
+      </c>
+      <c r="KZ246">
+        <f t="shared" si="555"/>
+        <v>332</v>
+      </c>
+      <c r="LA246">
+        <f t="shared" si="555"/>
+        <v>332</v>
+      </c>
+      <c r="LB246">
+        <f t="shared" si="555"/>
+        <v>332</v>
+      </c>
+      <c r="LC246">
+        <f t="shared" si="555"/>
+        <v>332</v>
+      </c>
+      <c r="LD246">
+        <f t="shared" si="555"/>
+        <v>332</v>
+      </c>
+      <c r="LE246">
+        <f t="shared" si="555"/>
+        <v>332</v>
+      </c>
+      <c r="LF246">
+        <f t="shared" si="555"/>
+        <v>332</v>
+      </c>
+      <c r="LG246">
+        <f t="shared" si="555"/>
+        <v>332</v>
+      </c>
+      <c r="LH246">
+        <f t="shared" si="555"/>
+        <v>332</v>
+      </c>
+      <c r="LI246">
+        <f t="shared" si="555"/>
+        <v>332</v>
+      </c>
+      <c r="LJ246">
+        <f t="shared" si="555"/>
+        <v>332</v>
+      </c>
+      <c r="LK246">
+        <f t="shared" si="555"/>
+        <v>332</v>
+      </c>
+      <c r="LL246">
+        <f t="shared" ref="LL246:NW246" si="556">MEDIAN(LL238:LL243)</f>
+        <v>332</v>
+      </c>
+      <c r="LM246">
+        <f t="shared" si="556"/>
+        <v>332</v>
+      </c>
+      <c r="LN246">
+        <f t="shared" si="556"/>
+        <v>332</v>
+      </c>
+      <c r="LO246">
+        <f t="shared" si="556"/>
+        <v>332</v>
+      </c>
+      <c r="LP246">
+        <f t="shared" si="556"/>
+        <v>332</v>
+      </c>
+      <c r="LQ246">
+        <f t="shared" si="556"/>
+        <v>332</v>
+      </c>
+      <c r="LR246">
+        <f t="shared" si="556"/>
+        <v>332</v>
+      </c>
+      <c r="LS246">
+        <f t="shared" si="556"/>
+        <v>332</v>
+      </c>
+      <c r="LT246">
+        <f t="shared" si="556"/>
+        <v>332</v>
+      </c>
+      <c r="LU246">
+        <f t="shared" si="556"/>
+        <v>332</v>
+      </c>
+      <c r="LV246">
+        <f t="shared" si="556"/>
+        <v>332</v>
+      </c>
+      <c r="LW246">
+        <f t="shared" si="556"/>
+        <v>332</v>
+      </c>
+      <c r="LX246">
+        <f t="shared" si="556"/>
+        <v>332</v>
+      </c>
+      <c r="LY246">
+        <f t="shared" si="556"/>
+        <v>332</v>
+      </c>
+      <c r="LZ246">
+        <f t="shared" si="556"/>
+        <v>332</v>
+      </c>
+      <c r="MA246">
+        <f t="shared" si="556"/>
+        <v>332</v>
+      </c>
+      <c r="MB246">
+        <f t="shared" si="556"/>
+        <v>332</v>
+      </c>
+      <c r="MC246">
+        <f t="shared" si="556"/>
+        <v>332</v>
+      </c>
+      <c r="MD246">
+        <f t="shared" si="556"/>
+        <v>332</v>
+      </c>
+      <c r="ME246">
+        <f t="shared" si="556"/>
+        <v>332</v>
+      </c>
+      <c r="MF246">
+        <f t="shared" si="556"/>
+        <v>332</v>
+      </c>
+      <c r="MG246">
+        <f t="shared" si="556"/>
+        <v>332</v>
+      </c>
+      <c r="MH246">
+        <f t="shared" si="556"/>
+        <v>332</v>
+      </c>
+      <c r="MI246">
+        <f t="shared" si="556"/>
+        <v>332</v>
+      </c>
+      <c r="MJ246">
+        <f t="shared" si="556"/>
+        <v>332</v>
+      </c>
+      <c r="MK246">
+        <f t="shared" si="556"/>
+        <v>332</v>
+      </c>
+      <c r="ML246">
+        <f t="shared" si="556"/>
+        <v>332</v>
+      </c>
+      <c r="MM246">
+        <f t="shared" si="556"/>
+        <v>332</v>
+      </c>
+      <c r="MN246">
+        <f t="shared" si="556"/>
+        <v>332</v>
+      </c>
+      <c r="MO246">
+        <f t="shared" si="556"/>
+        <v>332</v>
+      </c>
+      <c r="MP246">
+        <f t="shared" si="556"/>
+        <v>332</v>
+      </c>
+      <c r="MQ246">
+        <f t="shared" si="556"/>
+        <v>332</v>
+      </c>
+      <c r="MR246">
+        <f t="shared" si="556"/>
+        <v>332</v>
+      </c>
+      <c r="MS246">
+        <f t="shared" si="556"/>
+        <v>332</v>
+      </c>
+      <c r="MT246">
+        <f t="shared" si="556"/>
+        <v>332</v>
+      </c>
+      <c r="MU246">
+        <f t="shared" si="556"/>
+        <v>332</v>
+      </c>
+      <c r="MV246">
+        <f t="shared" si="556"/>
+        <v>332</v>
+      </c>
+      <c r="MW246">
+        <f t="shared" si="556"/>
+        <v>332</v>
+      </c>
+      <c r="MX246">
+        <f t="shared" si="556"/>
+        <v>332</v>
+      </c>
+      <c r="MY246">
+        <f t="shared" si="556"/>
+        <v>332</v>
+      </c>
+      <c r="MZ246">
+        <f t="shared" si="556"/>
+        <v>332</v>
+      </c>
+      <c r="NA246">
+        <f t="shared" si="556"/>
+        <v>332</v>
+      </c>
+      <c r="NB246">
+        <f t="shared" si="556"/>
+        <v>332</v>
+      </c>
+      <c r="NC246">
+        <f t="shared" si="556"/>
+        <v>332</v>
+      </c>
+      <c r="ND246">
+        <f t="shared" si="556"/>
+        <v>332</v>
+      </c>
+      <c r="NE246">
+        <f t="shared" si="556"/>
+        <v>332</v>
+      </c>
+      <c r="NF246">
+        <f t="shared" si="556"/>
+        <v>332</v>
+      </c>
+      <c r="NG246">
+        <f t="shared" si="556"/>
+        <v>332</v>
+      </c>
+      <c r="NH246">
+        <f t="shared" si="556"/>
+        <v>332</v>
+      </c>
+      <c r="NI246">
+        <f t="shared" si="556"/>
+        <v>332</v>
+      </c>
+      <c r="NJ246">
+        <f t="shared" si="556"/>
+        <v>332</v>
+      </c>
+      <c r="NK246">
+        <f t="shared" si="556"/>
+        <v>332</v>
+      </c>
+      <c r="NL246">
+        <f t="shared" si="556"/>
+        <v>332</v>
+      </c>
+      <c r="NM246">
+        <f t="shared" si="556"/>
+        <v>332</v>
+      </c>
+      <c r="NN246">
+        <f t="shared" si="556"/>
+        <v>332</v>
+      </c>
+      <c r="NO246">
+        <f t="shared" si="556"/>
+        <v>332</v>
+      </c>
+      <c r="NP246">
+        <f t="shared" si="556"/>
+        <v>332</v>
+      </c>
+      <c r="NQ246">
+        <f t="shared" si="556"/>
+        <v>332</v>
+      </c>
+      <c r="NR246">
+        <f t="shared" si="556"/>
+        <v>332</v>
+      </c>
+      <c r="NS246">
+        <f t="shared" si="556"/>
+        <v>332</v>
+      </c>
+      <c r="NT246">
+        <f t="shared" si="556"/>
+        <v>332</v>
+      </c>
+      <c r="NU246">
+        <f t="shared" si="556"/>
+        <v>332</v>
+      </c>
+      <c r="NV246">
+        <f t="shared" si="556"/>
+        <v>332</v>
+      </c>
+      <c r="NW246">
+        <f t="shared" si="556"/>
+        <v>332</v>
+      </c>
+      <c r="NX246">
+        <f t="shared" ref="NX246:QI246" si="557">MEDIAN(NX238:NX243)</f>
+        <v>332</v>
+      </c>
+      <c r="NY246">
+        <f t="shared" si="557"/>
+        <v>332</v>
+      </c>
+      <c r="NZ246">
+        <f t="shared" si="557"/>
+        <v>332</v>
+      </c>
+      <c r="OA246">
+        <f t="shared" si="557"/>
+        <v>332</v>
+      </c>
+      <c r="OB246">
+        <f t="shared" si="557"/>
+        <v>332</v>
+      </c>
+      <c r="OC246">
+        <f t="shared" si="557"/>
+        <v>332</v>
+      </c>
+      <c r="OD246">
+        <f t="shared" si="557"/>
+        <v>332</v>
+      </c>
+      <c r="OE246">
+        <f t="shared" si="557"/>
+        <v>332</v>
+      </c>
+      <c r="OF246">
+        <f t="shared" si="557"/>
+        <v>332</v>
+      </c>
+      <c r="OG246">
+        <f t="shared" si="557"/>
+        <v>332</v>
+      </c>
+      <c r="OH246">
+        <f t="shared" si="557"/>
+        <v>332</v>
+      </c>
+      <c r="OI246">
+        <f t="shared" si="557"/>
+        <v>332</v>
+      </c>
+      <c r="OJ246">
+        <f t="shared" si="557"/>
+        <v>332</v>
+      </c>
+      <c r="OK246">
+        <f t="shared" si="557"/>
+        <v>332</v>
+      </c>
+      <c r="OL246">
+        <f t="shared" si="557"/>
+        <v>332</v>
+      </c>
+      <c r="OM246">
+        <f t="shared" si="557"/>
+        <v>332</v>
+      </c>
+      <c r="ON246">
+        <f t="shared" si="557"/>
+        <v>332</v>
+      </c>
+      <c r="OO246">
+        <f t="shared" si="557"/>
+        <v>332</v>
+      </c>
+      <c r="OP246">
+        <f t="shared" si="557"/>
+        <v>332</v>
+      </c>
+      <c r="OQ246">
+        <f t="shared" si="557"/>
+        <v>332</v>
+      </c>
+      <c r="OR246">
+        <f t="shared" si="557"/>
+        <v>332</v>
+      </c>
+      <c r="OS246">
+        <f t="shared" si="557"/>
+        <v>332</v>
+      </c>
+      <c r="OT246">
+        <f t="shared" si="557"/>
+        <v>332</v>
+      </c>
+      <c r="OU246">
+        <f t="shared" si="557"/>
+        <v>332</v>
+      </c>
+      <c r="OV246">
+        <f t="shared" si="557"/>
+        <v>332</v>
+      </c>
+      <c r="OW246">
+        <f t="shared" si="557"/>
+        <v>332</v>
+      </c>
+      <c r="OX246">
+        <f t="shared" si="557"/>
+        <v>332</v>
+      </c>
+      <c r="OY246">
+        <f t="shared" si="557"/>
+        <v>332</v>
+      </c>
+      <c r="OZ246">
+        <f t="shared" si="557"/>
+        <v>332</v>
+      </c>
+      <c r="PA246">
+        <f t="shared" si="557"/>
+        <v>332</v>
+      </c>
+      <c r="PB246">
+        <f t="shared" si="557"/>
+        <v>332</v>
+      </c>
+      <c r="PC246">
+        <f t="shared" si="557"/>
+        <v>332</v>
+      </c>
+      <c r="PD246">
+        <f t="shared" si="557"/>
+        <v>332</v>
+      </c>
+      <c r="PE246">
+        <f t="shared" si="557"/>
+        <v>332</v>
+      </c>
+      <c r="PF246">
+        <f t="shared" si="557"/>
+        <v>332</v>
+      </c>
+      <c r="PG246">
+        <f t="shared" si="557"/>
+        <v>332</v>
+      </c>
+      <c r="PH246">
+        <f t="shared" si="557"/>
+        <v>332</v>
+      </c>
+      <c r="PI246">
+        <f t="shared" si="557"/>
+        <v>332</v>
+      </c>
+      <c r="PJ246">
+        <f t="shared" si="557"/>
+        <v>332</v>
+      </c>
+      <c r="PK246">
+        <f t="shared" si="557"/>
+        <v>332</v>
+      </c>
+      <c r="PL246">
+        <f t="shared" si="557"/>
+        <v>332</v>
+      </c>
+      <c r="PM246">
+        <f t="shared" si="557"/>
+        <v>332</v>
+      </c>
+      <c r="PN246">
+        <f t="shared" si="557"/>
+        <v>332</v>
+      </c>
+      <c r="PO246">
+        <f t="shared" si="557"/>
+        <v>332</v>
+      </c>
+      <c r="PP246">
+        <f t="shared" si="557"/>
+        <v>332</v>
+      </c>
+      <c r="PQ246">
+        <f t="shared" si="557"/>
+        <v>332</v>
+      </c>
+      <c r="PR246">
+        <f t="shared" si="557"/>
+        <v>332</v>
+      </c>
+      <c r="PS246">
+        <f t="shared" si="557"/>
+        <v>332</v>
+      </c>
+      <c r="PT246">
+        <f t="shared" si="557"/>
+        <v>332</v>
+      </c>
+      <c r="PU246">
+        <f t="shared" si="557"/>
+        <v>332</v>
+      </c>
+      <c r="PV246">
+        <f t="shared" si="557"/>
+        <v>332</v>
+      </c>
+      <c r="PW246">
+        <f t="shared" si="557"/>
+        <v>332</v>
+      </c>
+      <c r="PX246">
+        <f t="shared" si="557"/>
+        <v>332</v>
+      </c>
+      <c r="PY246">
+        <f t="shared" si="557"/>
+        <v>332</v>
+      </c>
+      <c r="PZ246">
+        <f t="shared" si="557"/>
+        <v>332</v>
+      </c>
+      <c r="QA246">
+        <f t="shared" si="557"/>
+        <v>332</v>
+      </c>
+      <c r="QB246">
+        <f t="shared" si="557"/>
+        <v>332</v>
+      </c>
+      <c r="QC246">
+        <f t="shared" si="557"/>
+        <v>332</v>
+      </c>
+      <c r="QD246">
+        <f t="shared" si="557"/>
+        <v>332</v>
+      </c>
+      <c r="QE246">
+        <f t="shared" si="557"/>
+        <v>332</v>
+      </c>
+      <c r="QF246">
+        <f t="shared" si="557"/>
+        <v>332</v>
+      </c>
+      <c r="QG246">
+        <f t="shared" si="557"/>
+        <v>332</v>
+      </c>
+      <c r="QH246">
+        <f t="shared" si="557"/>
+        <v>332</v>
+      </c>
+      <c r="QI246">
+        <f t="shared" si="557"/>
+        <v>332</v>
+      </c>
+      <c r="QJ246">
+        <f t="shared" ref="QJ246:SU246" si="558">MEDIAN(QJ238:QJ243)</f>
+        <v>332</v>
+      </c>
+      <c r="QK246">
+        <f t="shared" si="558"/>
+        <v>332</v>
+      </c>
+      <c r="QL246">
+        <f t="shared" si="558"/>
+        <v>332</v>
+      </c>
+      <c r="QM246">
+        <f t="shared" si="558"/>
+        <v>332</v>
+      </c>
+      <c r="QN246">
+        <f t="shared" si="558"/>
+        <v>332</v>
+      </c>
+      <c r="QO246">
+        <f t="shared" si="558"/>
+        <v>332</v>
+      </c>
+      <c r="QP246">
+        <f t="shared" si="558"/>
+        <v>332</v>
+      </c>
+      <c r="QQ246">
+        <f t="shared" si="558"/>
+        <v>332</v>
+      </c>
+      <c r="QR246">
+        <f t="shared" si="558"/>
+        <v>332</v>
+      </c>
+      <c r="QS246">
+        <f t="shared" si="558"/>
+        <v>332</v>
+      </c>
+      <c r="QT246">
+        <f t="shared" si="558"/>
+        <v>332</v>
+      </c>
+      <c r="QU246">
+        <f t="shared" si="558"/>
+        <v>332</v>
+      </c>
+      <c r="QV246">
+        <f t="shared" si="558"/>
+        <v>332</v>
+      </c>
+      <c r="QW246">
+        <f t="shared" si="558"/>
+        <v>332</v>
+      </c>
+      <c r="QX246">
+        <f t="shared" si="558"/>
+        <v>332</v>
+      </c>
+      <c r="QY246">
+        <f t="shared" si="558"/>
+        <v>332</v>
+      </c>
+      <c r="QZ246">
+        <f t="shared" si="558"/>
+        <v>332</v>
+      </c>
+      <c r="RA246">
+        <f t="shared" si="558"/>
+        <v>332</v>
+      </c>
+      <c r="RB246">
+        <f t="shared" si="558"/>
+        <v>332</v>
+      </c>
+      <c r="RC246">
+        <f t="shared" si="558"/>
+        <v>332</v>
+      </c>
+      <c r="RD246">
+        <f t="shared" si="558"/>
+        <v>332</v>
+      </c>
+      <c r="RE246">
+        <f t="shared" si="558"/>
+        <v>332</v>
+      </c>
+      <c r="RF246">
+        <f t="shared" si="558"/>
+        <v>332</v>
+      </c>
+      <c r="RG246">
+        <f t="shared" si="558"/>
+        <v>332</v>
+      </c>
+      <c r="RH246">
+        <f t="shared" si="558"/>
+        <v>332</v>
+      </c>
+      <c r="RI246">
+        <f t="shared" si="558"/>
+        <v>332</v>
+      </c>
+      <c r="RJ246">
+        <f t="shared" si="558"/>
+        <v>332</v>
+      </c>
+      <c r="RK246">
+        <f t="shared" si="558"/>
+        <v>332</v>
+      </c>
+      <c r="RL246">
+        <f t="shared" si="558"/>
+        <v>332</v>
+      </c>
+      <c r="RM246">
+        <f t="shared" si="558"/>
+        <v>332</v>
+      </c>
+      <c r="RN246">
+        <f t="shared" si="558"/>
+        <v>332</v>
+      </c>
+      <c r="RO246">
+        <f t="shared" si="558"/>
+        <v>332</v>
+      </c>
+      <c r="RP246">
+        <f t="shared" si="558"/>
+        <v>332</v>
+      </c>
+      <c r="RQ246">
+        <f t="shared" si="558"/>
+        <v>332</v>
+      </c>
+      <c r="RR246">
+        <f t="shared" si="558"/>
+        <v>332</v>
+      </c>
+      <c r="RS246">
+        <f t="shared" si="558"/>
+        <v>332</v>
+      </c>
+      <c r="RT246">
+        <f t="shared" si="558"/>
+        <v>332</v>
+      </c>
+      <c r="RU246">
+        <f t="shared" si="558"/>
+        <v>332</v>
+      </c>
+      <c r="RV246">
+        <f t="shared" si="558"/>
+        <v>332</v>
+      </c>
+      <c r="RW246">
+        <f t="shared" si="558"/>
+        <v>332</v>
+      </c>
+      <c r="RX246">
+        <f t="shared" si="558"/>
+        <v>332</v>
+      </c>
+      <c r="RY246">
+        <f t="shared" si="558"/>
+        <v>332</v>
+      </c>
+      <c r="RZ246">
+        <f t="shared" si="558"/>
+        <v>332</v>
+      </c>
+      <c r="SA246">
+        <f t="shared" si="558"/>
+        <v>332</v>
+      </c>
+      <c r="SB246">
+        <f t="shared" si="558"/>
+        <v>332</v>
+      </c>
+      <c r="SC246">
+        <f t="shared" si="558"/>
+        <v>332</v>
+      </c>
+      <c r="SD246">
+        <f t="shared" si="558"/>
+        <v>332</v>
+      </c>
+      <c r="SE246">
+        <f t="shared" si="558"/>
+        <v>332</v>
+      </c>
+      <c r="SF246">
+        <f t="shared" si="558"/>
+        <v>332</v>
+      </c>
+      <c r="SG246">
+        <f t="shared" si="558"/>
+        <v>332</v>
+      </c>
+      <c r="SH246">
+        <f t="shared" si="558"/>
+        <v>332</v>
+      </c>
+      <c r="SI246">
+        <f t="shared" si="558"/>
+        <v>332</v>
+      </c>
+      <c r="SJ246">
+        <f t="shared" si="558"/>
+        <v>332</v>
+      </c>
+      <c r="SK246">
+        <f t="shared" si="558"/>
+        <v>332</v>
+      </c>
+      <c r="SL246">
+        <f t="shared" si="558"/>
+        <v>332</v>
+      </c>
+      <c r="SM246">
+        <f t="shared" si="558"/>
+        <v>332</v>
+      </c>
+      <c r="SN246">
+        <f t="shared" si="558"/>
+        <v>332</v>
+      </c>
+      <c r="SO246">
+        <f t="shared" si="558"/>
+        <v>332</v>
+      </c>
+      <c r="SP246">
+        <f t="shared" si="558"/>
+        <v>332</v>
+      </c>
+      <c r="SQ246">
+        <f t="shared" si="558"/>
+        <v>332</v>
+      </c>
+      <c r="SR246">
+        <f t="shared" si="558"/>
+        <v>332</v>
+      </c>
+      <c r="SS246">
+        <f t="shared" si="558"/>
+        <v>332</v>
+      </c>
+      <c r="ST246">
+        <f t="shared" si="558"/>
+        <v>332</v>
+      </c>
+      <c r="SU246">
+        <f t="shared" si="558"/>
+        <v>332</v>
+      </c>
+      <c r="SV246">
+        <f t="shared" ref="SV246:SZ246" si="559">MEDIAN(SV238:SV243)</f>
+        <v>332</v>
+      </c>
+      <c r="SW246">
+        <f t="shared" si="559"/>
+        <v>332</v>
+      </c>
+      <c r="SX246">
+        <f t="shared" si="559"/>
+        <v>332</v>
+      </c>
+      <c r="SY246">
+        <f t="shared" si="559"/>
+        <v>332</v>
+      </c>
+      <c r="SZ246">
+        <f t="shared" si="559"/>
+        <v>332</v>
+      </c>
+    </row>
+    <row r="247" spans="2:520" x14ac:dyDescent="0.25">
+      <c r="C247">
+        <f>C246/(332)</f>
+        <v>0.71084337349397586</v>
       </c>
     </row>
   </sheetData>

</xml_diff>